<commit_message>
added impl profile metadata
</commit_message>
<xml_diff>
--- a/internal/message flows.xlsx
+++ b/internal/message flows.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="23380" yWindow="1420" windowWidth="25840" windowHeight="20380" tabRatio="500"/>
+    <workbookView xWindow="23380" yWindow="1420" windowWidth="25840" windowHeight="20380" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Impl-MFBAuthN" sheetId="1" r:id="rId1"/>
     <sheet name="Impl-MFB-Enc" sheetId="2" r:id="rId2"/>
     <sheet name="Depl-MFB-Authn" sheetId="3" r:id="rId3"/>
     <sheet name="Depl-MFB-Enc" sheetId="4" r:id="rId4"/>
+    <sheet name="04 MD" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="97">
   <si>
     <t>SP</t>
   </si>
@@ -244,13 +245,100 @@
   </si>
   <si>
     <t>Assertion Query AttributeQuery</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">MUST support the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Courier New"/>
+      </rPr>
+      <t>&lt;ds:X509Certificate&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+      </rPr>
+      <t xml:space="preserve"> element as key representation int the &lt;md:KeyDescriptor&gt; element</t>
+    </r>
+  </si>
+  <si>
+    <t>Support for other key representations than &lt;ds:X509Certificate&gt;, and for other mechanisms for credential distribution, is OPTIONAL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implementations MUST support some form of path validation of signing, TLS, and encryption credentials used to secure SAML exchanges against one or more trusted certificate authorities. </t>
+  </si>
+  <si>
+    <t>[SAML2Meta]</t>
+  </si>
+  <si>
+    <t>Support for PKIX [RFC5280] is RECOMMENDED; implementations SHOULD document the behavior of the validation mechanisms they employ, particular with respect to limitations or divergence from PKIX [RFC5280]</t>
+  </si>
+  <si>
+    <t>Implementations MUST support the use of OCSP [RFC2560] and Certificate Revocation Lists (CRLs) obtained via the "CRL Distribution Point" X.509 extension [RFC5280] for revocation checking of those credentials.</t>
+  </si>
+  <si>
+    <t>Implementations MAY support additional constraints on the contents of certificates used by particular entities, such as "subjectAltName" or "DN", key usage constraints, or policy extensions, but SHOULD document such features and make them optional to enable where possible.</t>
+  </si>
+  <si>
+    <t>[MetaAttr]</t>
+  </si>
+  <si>
+    <t>Implementations SHOULD support the SAML V2.0 Metadata Extension for Entity Attributes Version 1.0 [MetaAttr] and provide policy controls on the basis of SAML attributes supplied via this extension mechanism.</t>
+  </si>
+  <si>
+    <t>eGov 2.0</t>
+  </si>
+  <si>
+    <t>Dispostiion</t>
+  </si>
+  <si>
+    <t>MUST support SAML V2.0 Metadata [SAML2MD] as updated by Errata [SAML2Errata]</t>
+  </si>
+  <si>
+    <t>MUST support SAML V2.0 Metadata Schema [SAML2MD-xsd]</t>
+  </si>
+  <si>
+    <t>Implementations MUST support the SAML V2.0 Metadata Interoperability Profile Version 1.0 [SAML2MDIOP].</t>
+  </si>
+  <si>
+    <t>[SAML2MDIOP]</t>
+  </si>
+  <si>
+    <t>[SAML2MD-xsd]</t>
+  </si>
+  <si>
+    <t>[SAML2MD]</t>
+  </si>
+  <si>
+    <t>new</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>Support for the generation or exportation of metadata is OPTIONAL.</t>
+  </si>
+  <si>
+    <t>Implementations MUST support the publication of metadata using the Well-Known-Location method defined in section 4.1 of [SAML2Meta] (under the assumption that entityID values used are suitable for such support).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -290,6 +378,16 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -308,7 +406,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="339">
+  <cellStyleXfs count="365">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -648,8 +746,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -676,8 +800,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="339">
+  <cellStyles count="365">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
@@ -847,6 +980,19 @@
     <cellStyle name="Besuchter Link" xfId="334" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="336" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="338" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="340" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="342" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="344" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="346" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="348" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="350" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="352" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="354" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="356" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="358" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="360" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="362" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="364" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
@@ -1016,6 +1162,19 @@
     <cellStyle name="Link" xfId="333" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="335" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="337" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="339" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="341" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="343" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="345" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="347" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="349" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="351" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="353" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="355" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="357" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="359" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="361" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1347,7 +1506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
@@ -2483,7 +2642,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="3">
-        <f t="shared" ref="A4:A9" si="1">A3+1</f>
+        <f t="shared" ref="A4:A8" si="1">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="3" t="str">
@@ -2742,7 +2901,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="B1:G4"/>
+      <selection sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2883,4 +3042,397 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4" style="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" style="12" customWidth="1"/>
+    <col min="8" max="8" width="108.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1">
+        <v>100</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>CONCATENATE("MDP-",A2)</f>
+        <v>MDP-100</v>
+      </c>
+      <c r="C2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="14" customHeight="1">
+      <c r="A3" s="1">
+        <f>A2+1</f>
+        <v>101</v>
+      </c>
+      <c r="B3" s="1" t="str">
+        <f t="shared" ref="B3:B19" si="0">CONCATENATE("MDP-",A3)</f>
+        <v>MDP-101</v>
+      </c>
+      <c r="C3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E3" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="H3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1">
+        <f t="shared" ref="A4:A19" si="1">A3+1</f>
+        <v>102</v>
+      </c>
+      <c r="B4" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-102</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="12">
+        <v>163</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="16">
+      <c r="A5" s="1">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-103</v>
+      </c>
+      <c r="C5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="12">
+        <v>167</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-104</v>
+      </c>
+      <c r="C6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="12">
+        <v>168</v>
+      </c>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="1">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-105</v>
+      </c>
+      <c r="C7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="12">
+        <v>170</v>
+      </c>
+      <c r="H7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="1">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+      <c r="B8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-106</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="12">
+        <v>172</v>
+      </c>
+      <c r="H8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" s="1">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+      <c r="B9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-107</v>
+      </c>
+      <c r="D9" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="12">
+        <v>176</v>
+      </c>
+      <c r="H9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" s="1">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+      <c r="B10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-108</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10" s="12">
+        <v>179</v>
+      </c>
+      <c r="H10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" s="1">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="B11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-109</v>
+      </c>
+      <c r="C11" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F11" s="12">
+        <v>186</v>
+      </c>
+      <c r="H11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-110</v>
+      </c>
+      <c r="F12" s="12">
+        <v>190</v>
+      </c>
+      <c r="H12" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="A13" s="1">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-111</v>
+      </c>
+      <c r="F13" s="12">
+        <v>191</v>
+      </c>
+      <c r="H13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="B14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-112</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="B15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+      <c r="B16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="1">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+      <c r="B17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-115</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="1">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+      <c r="B18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="1">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+      <c r="B19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>MDP-117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>